<commit_message>
Update Bill of Materials - Hypnos V2.xlsx
Update the right part for 100k ohm resistor
</commit_message>
<xml_diff>
--- a/Hypnos/Bill of Materials - Hypnos V2.xlsx
+++ b/Hypnos/Bill of Materials - Hypnos V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao Nguyen\Desktop\OpenSLab\eDNA\Power Board\3v3 Hypnos\Final for V2\Updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B70DE2-12A8-446D-BF5E-DF9FE6A71BCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73B6402-4879-4982-8AEA-C99D3C5575DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="77">
   <si>
     <t>Digikey</t>
   </si>
@@ -188,9 +188,6 @@
     <t>100k resistor 1%</t>
   </si>
   <si>
-    <t>311-100KCRCT-ND</t>
-  </si>
-  <si>
     <t>6.2k ohm resistor 1%</t>
   </si>
   <si>
@@ -258,6 +255,15 @@
   </si>
   <si>
     <t>279-CRGCQ1206J10K</t>
+  </si>
+  <si>
+    <t>311-100KFRCT-ND</t>
+  </si>
+  <si>
+    <t>RC1206FR-07100KL</t>
+  </si>
+  <si>
+    <t>603-RC1206FR-07100KL</t>
   </si>
 </sst>
 </file>
@@ -755,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -799,13 +805,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>56</v>
-      </c>
-      <c r="C2" s="10">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>57</v>
       </c>
       <c r="E2" s="10">
         <v>0.17</v>
@@ -815,7 +821,7 @@
         <v>0.17</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -845,7 +851,7 @@
         <v>0.66</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -872,13 +878,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="14">
         <v>1</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5" s="14">
         <v>0.1</v>
@@ -887,7 +893,7 @@
         <v>0.1</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -897,7 +903,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -907,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="E6" s="14">
         <v>0.1</v>
@@ -917,7 +923,7 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -947,7 +953,7 @@
         <v>0.4</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -977,7 +983,7 @@
         <v>1.95</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -1005,7 +1011,7 @@
         <v>8.77</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -1046,7 +1052,7 @@
         <v>0.68</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
@@ -1076,7 +1082,7 @@
         <v>0.91</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -1104,7 +1110,7 @@
         <v>0.2</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
@@ -1134,7 +1140,7 @@
         <v>0.38</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -1164,7 +1170,7 @@
         <v>1.02</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -1178,13 +1184,13 @@
         <v>0</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" s="10">
-        <v>1</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="E16" s="10">
         <v>0.1</v>
@@ -1194,7 +1200,7 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1208,13 +1214,13 @@
         <v>0</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="10">
+        <v>1</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="C17" s="10">
-        <v>1</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="E17" s="10">
         <v>0.1</v>
@@ -1224,7 +1230,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
@@ -1238,13 +1244,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="C18" s="10">
-        <v>1</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="E18" s="10">
         <v>0.1</v>
@@ -1254,7 +1260,7 @@
         <v>0.1</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -1311,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B778148E-242D-409E-9127-666EF26A5862}">
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1359,13 +1365,13 @@
         <v>31</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="10">
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="10">
         <v>0.15</v>
@@ -1375,7 +1381,7 @@
         <v>0.15</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
@@ -1403,11 +1409,11 @@
         <v>0.31</v>
       </c>
       <c r="F3" s="21">
-        <f t="shared" ref="F3:F14" si="0">C3*E3</f>
+        <f t="shared" ref="F3:F15" si="0">C3*E3</f>
         <v>0.62</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
@@ -1438,13 +1444,13 @@
         <v>31</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="14">
         <v>1</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="14">
         <v>0.09</v>
@@ -1454,7 +1460,7 @@
         <v>0.09</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -1463,209 +1469,207 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C6" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="E6" s="14">
         <v>0.1</v>
       </c>
       <c r="F6" s="14">
-        <f t="shared" ref="F6:F8" si="1">E6*C6</f>
-        <v>0.4</v>
+        <f t="shared" ref="F6" si="1">E6*C6</f>
+        <v>0.2</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="16">
-        <v>1206</v>
-      </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
+      <c r="K6" s="17" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="14">
-        <v>1</v>
-      </c>
-      <c r="D7" s="24">
-        <v>1660</v>
+        <v>4</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="E7" s="14">
-        <v>2.3199999999999998</v>
+        <v>0.1</v>
       </c>
       <c r="F7" s="14">
-        <f t="shared" si="1"/>
-        <v>2.3199999999999998</v>
+        <f t="shared" ref="F7:F9" si="2">E7*C7</f>
+        <v>0.4</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="16"/>
+      <c r="K7" s="16">
+        <v>1206</v>
+      </c>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C8" s="14">
         <v>1</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>15</v>
+      <c r="D8" s="24">
+        <v>1660</v>
       </c>
       <c r="E8" s="14">
-        <v>8.77</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="F8" s="14">
-        <f t="shared" si="1"/>
-        <v>8.77</v>
+        <f t="shared" si="2"/>
+        <v>2.3199999999999998</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
       <c r="K8" s="16"/>
-      <c r="L8" s="14" t="s">
-        <v>45</v>
-      </c>
+      <c r="L8" s="14"/>
       <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="14"/>
+      <c r="A9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="14">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="14">
+        <v>8.77</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="2"/>
+        <v>8.77</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>57</v>
+      </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="16"/>
-      <c r="L9" s="14"/>
+      <c r="L9" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="14">
-        <v>2</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="14">
-        <v>0.33</v>
-      </c>
-      <c r="F10" s="21">
-        <f t="shared" si="0"/>
-        <v>0.66</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
-      <c r="K10" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="K10" s="16"/>
       <c r="L10" s="14"/>
       <c r="M10" s="14"/>
     </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>35</v>
+        <v>2</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="E11" s="14">
-        <v>0.91</v>
+        <v>0.33</v>
       </c>
       <c r="F11" s="21">
         <f t="shared" si="0"/>
-        <v>0.91</v>
+        <v>0.66</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="14" t="s">
-        <v>49</v>
-      </c>
+      <c r="K11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="14"/>
       <c r="M11" s="14"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" s="14">
-        <v>2</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>35</v>
       </c>
       <c r="E12" s="14">
-        <v>0.18</v>
+        <v>0.91</v>
       </c>
       <c r="F12" s="21">
         <f t="shared" si="0"/>
-        <v>0.36</v>
+        <v>0.91</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="16">
-        <v>1206</v>
-      </c>
-      <c r="L12" s="14"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="14" t="s">
+        <v>49</v>
+      </c>
       <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1673,29 +1677,29 @@
         <v>31</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C13" s="14">
         <v>2</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>37</v>
+      <c r="D13" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="E13" s="14">
-        <v>0.43</v>
+        <v>0.18</v>
       </c>
       <c r="F13" s="21">
         <f t="shared" si="0"/>
-        <v>0.86</v>
+        <v>0.36</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
-      <c r="K13" s="17" t="s">
-        <v>27</v>
+      <c r="K13" s="16">
+        <v>1206</v>
       </c>
       <c r="L13" s="14"/>
       <c r="M13" s="14"/>
@@ -1705,77 +1709,77 @@
         <v>31</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C14" s="14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="E14" s="14">
-        <v>0.1</v>
+        <v>0.43</v>
       </c>
       <c r="F14" s="21">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.86</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
       <c r="K14" s="17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L14" s="14"/>
       <c r="M14" s="14"/>
     </row>
-    <row r="15" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="10">
-        <v>1</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="10">
-        <f>E15*C15</f>
+      <c r="B15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="21">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
     </row>
     <row r="16" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="10">
         <v>1</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E16" s="10">
         <v>0.1</v>
@@ -1785,7 +1789,7 @@
         <v>0.1</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1801,13 +1805,13 @@
         <v>31</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C17" s="10">
         <v>1</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E17" s="10">
         <v>0.1</v>
@@ -1816,64 +1820,98 @@
         <f>E17*C17</f>
         <v>0.1</v>
       </c>
-      <c r="G17" s="18" t="s">
-        <v>58</v>
+      <c r="G17" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
       <c r="K17" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="10">
+        <f>E18*C18</f>
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="14">
-        <f>SUM(F2:F15)</f>
-        <v>15.339999999999998</v>
-      </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
+      <c r="F19" s="14">
+        <f>SUM(F2:F16)</f>
+        <v>15.539999999999997</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{59EA1C62-5141-47E4-849E-21AC47E6E96D}"/>
-    <hyperlink ref="A6" r:id="rId2" xr:uid="{647823C0-0146-41B6-8A0D-60E9F15E0075}"/>
-    <hyperlink ref="A7" r:id="rId3" xr:uid="{4049924F-283E-4A8D-A90B-3DA37B62CD35}"/>
-    <hyperlink ref="A8" r:id="rId4" xr:uid="{978AB516-90C8-4DBD-9CF5-43C75CD07F9C}"/>
-    <hyperlink ref="A12" r:id="rId5" xr:uid="{805A8BCB-C8CB-4492-BC3F-B7D52E5D08D3}"/>
-    <hyperlink ref="A11" r:id="rId6" xr:uid="{84AC990C-36C4-486B-B250-73A7C7181DD9}"/>
-    <hyperlink ref="A10" r:id="rId7" xr:uid="{AE2EDDDE-F74F-44AA-901A-D298D6F8F2DD}"/>
-    <hyperlink ref="A13" r:id="rId8" xr:uid="{42E8108F-FDFB-4CC6-AD39-9B7030DB41DE}"/>
-    <hyperlink ref="A14" r:id="rId9" xr:uid="{AED813D1-3494-4C52-8F98-7771FC767235}"/>
-    <hyperlink ref="A15" r:id="rId10" xr:uid="{26BE62CE-01A5-40F1-982D-1EBD6A03531A}"/>
-    <hyperlink ref="A16" r:id="rId11" xr:uid="{B6274010-BFC7-4EC1-96DB-E7F00B18BD53}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{647823C0-0146-41B6-8A0D-60E9F15E0075}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{4049924F-283E-4A8D-A90B-3DA37B62CD35}"/>
+    <hyperlink ref="A9" r:id="rId4" xr:uid="{978AB516-90C8-4DBD-9CF5-43C75CD07F9C}"/>
+    <hyperlink ref="A13" r:id="rId5" xr:uid="{805A8BCB-C8CB-4492-BC3F-B7D52E5D08D3}"/>
+    <hyperlink ref="A12" r:id="rId6" xr:uid="{84AC990C-36C4-486B-B250-73A7C7181DD9}"/>
+    <hyperlink ref="A11" r:id="rId7" xr:uid="{AE2EDDDE-F74F-44AA-901A-D298D6F8F2DD}"/>
+    <hyperlink ref="A14" r:id="rId8" xr:uid="{42E8108F-FDFB-4CC6-AD39-9B7030DB41DE}"/>
+    <hyperlink ref="A15" r:id="rId9" xr:uid="{AED813D1-3494-4C52-8F98-7771FC767235}"/>
+    <hyperlink ref="A16" r:id="rId10" xr:uid="{26BE62CE-01A5-40F1-982D-1EBD6A03531A}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{B6274010-BFC7-4EC1-96DB-E7F00B18BD53}"/>
     <hyperlink ref="A2" r:id="rId12" xr:uid="{DA8FF8F9-9FB0-473C-A3CB-0E87378BBBB1}"/>
     <hyperlink ref="A5" r:id="rId13" xr:uid="{9C6E4F96-280A-46C9-BA71-597D00B079AB}"/>
-    <hyperlink ref="A17" r:id="rId14" xr:uid="{625D3745-5C61-4FB0-A9AB-D10D529022E5}"/>
+    <hyperlink ref="A18" r:id="rId14" xr:uid="{625D3745-5C61-4FB0-A9AB-D10D529022E5}"/>
+    <hyperlink ref="A6" r:id="rId15" xr:uid="{B7345DB3-643B-4F6C-A4E0-36C293BC0632}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00EFBA5-BB63-4E95-AAB6-77207EAA5FF2}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1917,13 +1955,13 @@
         <v>39</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="29">
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="29">
         <v>0.16</v>
@@ -1933,7 +1971,7 @@
         <v>0.16</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
@@ -1959,7 +1997,7 @@
         <v>0.33</v>
       </c>
       <c r="F3" s="25">
-        <f t="shared" ref="F3:F11" si="0">E3*C3</f>
+        <f t="shared" ref="F3:F9" si="0">E3*C3</f>
         <v>0.66</v>
       </c>
       <c r="G3" s="25"/>
@@ -1988,13 +2026,13 @@
         <v>39</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="E5" s="14">
         <v>0.12</v>
@@ -2004,7 +2042,7 @@
         <v>0.12</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
@@ -2013,79 +2051,83 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" ref="F6" si="1">E6*C6</f>
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C7" s="25">
         <v>4</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="25">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" ref="F6:F7" si="1">E6*C6</f>
+      <c r="D7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="25">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" ref="F7:F8" si="2">E7*C7</f>
         <v>0.4</v>
-      </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="26">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="25">
-        <v>1</v>
-      </c>
-      <c r="D7" s="24">
-        <v>1660</v>
-      </c>
-      <c r="E7" s="25">
-        <v>1.95</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="1"/>
-        <v>1.95</v>
       </c>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
+      <c r="K7" s="26">
+        <v>1206</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C8" s="25">
         <v>1</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>41</v>
+      <c r="D8" s="24">
+        <v>1660</v>
       </c>
       <c r="E8" s="25">
-        <v>9.0399999999999991</v>
-      </c>
-      <c r="F8" s="27">
-        <f t="shared" si="0"/>
-        <v>9.0399999999999991</v>
+        <v>1.95</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="2"/>
+        <v>1.95</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
@@ -2094,12 +2136,25 @@
       <c r="K8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="27"/>
+      <c r="A9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="25">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="25">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="F9" s="27">
+        <f t="shared" si="0"/>
+        <v>9.0399999999999991</v>
+      </c>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
       <c r="I9" s="25"/>
@@ -2107,110 +2162,95 @@
       <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="25">
-        <v>0.34</v>
-      </c>
-      <c r="F10" s="27">
-        <f>E10*C10</f>
-        <v>0.68</v>
-      </c>
+      <c r="A10" s="13"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
       <c r="J10" s="25"/>
-      <c r="K10" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="25">
-        <v>1</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="E11" s="25">
-        <v>0.91</v>
-      </c>
-      <c r="F11" s="29">
-        <f t="shared" ref="F11:F14" si="2">E11*C11</f>
-        <v>0.91</v>
+        <v>0.34</v>
+      </c>
+      <c r="F11" s="27">
+        <f>E11*C11</f>
+        <v>0.68</v>
       </c>
       <c r="G11" s="25"/>
       <c r="H11" s="25"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
-      <c r="K11" s="26"/>
-    </row>
-    <row r="12" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="K11" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="25">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0.91</v>
+      </c>
+      <c r="F12" s="29">
+        <f t="shared" ref="F12:F15" si="3">E12*C12</f>
+        <v>0.91</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="34">
+      <c r="C13" s="29"/>
+      <c r="D13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="34">
         <v>0.15</v>
       </c>
-      <c r="F12" s="29">
-        <f t="shared" si="2"/>
+      <c r="F13" s="29">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="33">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="25">
-        <v>2</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="25">
-        <v>0.26</v>
-      </c>
-      <c r="F13" s="29">
-        <f t="shared" si="2"/>
-        <v>0.52</v>
-      </c>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26">
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="33">
         <v>1206</v>
       </c>
     </row>
@@ -2219,57 +2259,55 @@
         <v>39</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C14" s="25">
         <v>2</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>46</v>
+      <c r="D14" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="E14" s="25">
-        <v>0.5</v>
+        <v>0.26</v>
       </c>
       <c r="F14" s="29">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0.52</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="25"/>
       <c r="J14" s="25"/>
-      <c r="K14" s="28" t="s">
+      <c r="K14" s="26">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="25">
+        <v>2</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="28" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="29">
-        <v>1</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="29">
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="29">
-        <f>E15*C15</f>
-        <v>0.1</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2277,7 +2315,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="29">
         <v>1</v>
@@ -2286,14 +2324,14 @@
         <v>72</v>
       </c>
       <c r="E16" s="29">
-        <v>0.23</v>
+        <v>0.1</v>
       </c>
       <c r="F16" s="29">
         <f>E16*C16</f>
-        <v>0.23</v>
+        <v>0.1</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
@@ -2307,7 +2345,7 @@
         <v>39</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C17" s="29">
         <v>1</v>
@@ -2316,51 +2354,68 @@
         <v>71</v>
       </c>
       <c r="E17" s="29">
-        <v>0.1</v>
+        <v>0.23</v>
       </c>
       <c r="F17" s="29">
         <f>E17*C17</f>
-        <v>0.1</v>
-      </c>
-      <c r="G17" s="27" t="s">
-        <v>58</v>
+        <v>0.23</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>57</v>
       </c>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
       <c r="K17" s="30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="29">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="29">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="29">
+        <f>E18*C18</f>
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="25">
-        <f>SUM(F2:F16)</f>
-        <v>15.769999999999998</v>
-      </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="E19" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="25">
+        <f>SUM(F2:F17)</f>
+        <v>15.969999999999999</v>
+      </c>
       <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="H19" s="25" t="s">
+        <v>48</v>
+      </c>
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
@@ -2379,9 +2434,7 @@
       <c r="K20" s="25"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="25" t="s">
-        <v>44</v>
-      </c>
+      <c r="A21" s="25"/>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
       <c r="D21" s="25"/>
@@ -2394,7 +2447,9 @@
       <c r="K21" s="25"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="25"/>
+      <c r="A22" s="25" t="s">
+        <v>44</v>
+      </c>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
@@ -2406,22 +2461,36 @@
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
     </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{215EA094-C930-473B-BE4A-ADAAB4D5D66C}"/>
-    <hyperlink ref="A6" r:id="rId2" xr:uid="{70A97707-F1F6-4EFE-AB7E-31EBE6E57D86}"/>
-    <hyperlink ref="A7" r:id="rId3" xr:uid="{F2453D02-8024-44BD-9075-9396719F3556}"/>
-    <hyperlink ref="A8" r:id="rId4" xr:uid="{61F0098F-D0B4-4B63-A630-9DEAE7FCD7F7}"/>
-    <hyperlink ref="A13" r:id="rId5" xr:uid="{47DA31C5-C468-4690-AA2D-D92F08C147F2}"/>
-    <hyperlink ref="A11" r:id="rId6" xr:uid="{4555CB3D-A851-48FD-BF08-0C43F5DBE24A}"/>
-    <hyperlink ref="A10" r:id="rId7" xr:uid="{0CDDE590-1C19-404B-8E18-2F46E3425830}"/>
-    <hyperlink ref="A12" r:id="rId8" xr:uid="{C117FDDE-54F0-4BBA-8BC9-9DDA0464E7FD}"/>
-    <hyperlink ref="A14" r:id="rId9" xr:uid="{622C20A2-D84C-4CBE-AF23-27AB45B41F98}"/>
-    <hyperlink ref="A15" r:id="rId10" xr:uid="{A108A468-6EF0-42A4-97AF-3AB2DC7819C7}"/>
-    <hyperlink ref="A16" r:id="rId11" xr:uid="{3B3E04B3-5320-435D-A028-6452EB24F2D1}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{70A97707-F1F6-4EFE-AB7E-31EBE6E57D86}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{F2453D02-8024-44BD-9075-9396719F3556}"/>
+    <hyperlink ref="A9" r:id="rId4" xr:uid="{61F0098F-D0B4-4B63-A630-9DEAE7FCD7F7}"/>
+    <hyperlink ref="A14" r:id="rId5" xr:uid="{47DA31C5-C468-4690-AA2D-D92F08C147F2}"/>
+    <hyperlink ref="A12" r:id="rId6" xr:uid="{4555CB3D-A851-48FD-BF08-0C43F5DBE24A}"/>
+    <hyperlink ref="A11" r:id="rId7" xr:uid="{0CDDE590-1C19-404B-8E18-2F46E3425830}"/>
+    <hyperlink ref="A13" r:id="rId8" xr:uid="{C117FDDE-54F0-4BBA-8BC9-9DDA0464E7FD}"/>
+    <hyperlink ref="A15" r:id="rId9" xr:uid="{622C20A2-D84C-4CBE-AF23-27AB45B41F98}"/>
+    <hyperlink ref="A16" r:id="rId10" xr:uid="{A108A468-6EF0-42A4-97AF-3AB2DC7819C7}"/>
+    <hyperlink ref="A17" r:id="rId11" xr:uid="{3B3E04B3-5320-435D-A028-6452EB24F2D1}"/>
     <hyperlink ref="A2" r:id="rId12" xr:uid="{02C4B501-85F6-4FB2-95B4-BDAD90F7B1AA}"/>
-    <hyperlink ref="A17" r:id="rId13" xr:uid="{67F11B28-2656-4AB0-BA20-AC85BB219676}"/>
+    <hyperlink ref="A18" r:id="rId13" xr:uid="{67F11B28-2656-4AB0-BA20-AC85BB219676}"/>
     <hyperlink ref="A5" r:id="rId14" xr:uid="{E0EE49D4-0D5D-4FCB-ABA4-35155A815A3F}"/>
+    <hyperlink ref="A6" r:id="rId15" xr:uid="{0EE3201D-43B0-4228-AC4C-4DB6099FB31B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Bill of Material Hypnos V2
Correction to 100pF Part ID Digikey
</commit_message>
<xml_diff>
--- a/Hypnos/Bill of Materials - Hypnos V2.xlsx
+++ b/Hypnos/Bill of Materials - Hypnos V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao Nguyen\Desktop\OpenSLab\eDNA\Power Board\3v3 Hypnos\Final for V2\Updated\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao Nguyen\Documents\GitHub\OPEnS-Power\Hypnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73B6402-4879-4982-8AEA-C99D3C5575DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327CA54E-3CC8-45CA-94DE-A630F6E0759B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Mouser" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -212,9 +213,6 @@
     <t>100pF Capacitor</t>
   </si>
   <si>
-    <t>399-1205-1-ND</t>
-  </si>
-  <si>
     <t>A129833CT-ND</t>
   </si>
   <si>
@@ -264,6 +262,9 @@
   </si>
   <si>
     <t>603-RC1206FR-07100KL</t>
+  </si>
+  <si>
+    <t>399-1122-1-ND</t>
   </si>
 </sst>
 </file>
@@ -761,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -878,13 +879,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="14">
         <v>1</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="14">
         <v>0.1</v>
@@ -913,7 +914,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="14">
         <v>0.1</v>
@@ -1250,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E18" s="10">
         <v>0.1</v>
@@ -1320,7 +1321,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10">
         <v>0.15</v>
@@ -1444,13 +1445,13 @@
         <v>31</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="14">
         <v>1</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="14">
         <v>0.09</v>
@@ -1480,7 +1481,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="14">
         <v>0.1</v>
@@ -1779,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E16" s="10">
         <v>0.1</v>
@@ -1811,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="10">
         <v>0.1</v>
@@ -1843,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="10">
         <v>0.1</v>
@@ -1910,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00EFBA5-BB63-4E95-AAB6-77207EAA5FF2}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1961,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="29">
         <v>0.16</v>
@@ -2026,13 +2027,13 @@
         <v>39</v>
       </c>
       <c r="B5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>69</v>
       </c>
       <c r="E5" s="14">
         <v>0.12</v>
@@ -2062,7 +2063,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="14">
         <v>0.1</v>
@@ -2092,7 +2093,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="25">
         <v>0.1</v>
@@ -2237,7 +2238,7 @@
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="34">
         <v>0.15</v>
@@ -2321,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="29">
         <v>0.1</v>
@@ -2351,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" s="29">
         <v>0.23</v>
@@ -2381,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E18" s="29">
         <v>0.1</v>

</xml_diff>

<commit_message>
Hypnos V3 hardware fix
Added diode to Hypnos V3 to minimize leaking current from uSD card to 3VRAIL.
Add pdf for schematic Hypnos V2 + Hypnos V3
Updated bill of material to Hypnos V3
</commit_message>
<xml_diff>
--- a/Hypnos/Bill of Materials - Hypnos V2.xlsx
+++ b/Hypnos/Bill of Materials - Hypnos V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bao Nguyen\Documents\GitHub\OPEnS-Power\Hypnos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4BCDDF-3E85-4FB1-B66C-584BAC4CB669}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513C0783-F7BD-41A2-9BFA-B00C7B876134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="348" yWindow="756" windowWidth="3360" windowHeight="9420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Digikey" sheetId="1" r:id="rId1"/>
@@ -761,7 +761,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -923,7 +923,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>11</v>
@@ -933,7 +933,7 @@
       </c>
       <c r="F7" s="18">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>55</v>
@@ -1289,7 +1289,7 @@
       </c>
       <c r="F20" s="25">
         <f>SUM(F2:F19)</f>
-        <v>16.079999999999998</v>
+        <v>15.879999999999997</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1333,7 +1333,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,7 +1503,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>32</v>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="F7" s="14">
         <f t="shared" ref="F7:F9" si="2">E7*C7</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>55</v>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="F20" s="14">
         <f>SUM(F2:F19)</f>
-        <v>16.169999999999998</v>
+        <v>15.969999999999997</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -1937,7 +1937,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2098,7 +2098,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>61</v>
@@ -2108,7 +2108,7 @@
       </c>
       <c r="F7" s="14">
         <f t="shared" ref="F7:F8" si="2">E7*C7</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>55</v>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="F20" s="25">
         <f>SUM(F2:F19)</f>
-        <v>16.690000000000001</v>
+        <v>16.490000000000002</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="25" t="s">

</xml_diff>